<commit_message>
Minimal changes of ui
</commit_message>
<xml_diff>
--- a/Examples/TAU/DEGs.xlsx
+++ b/Examples/TAU/DEGs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikae\Desktop\MSc_Molecular_Biomedicine\Master_Thesis_Pavlopoulos\NAP\NORMA_project\Examples\TAU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8017DE3-B47E-424F-94E9-5A0E6C70C886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C89367-C8D9-4E7A-9CDF-9546C529D771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="3360" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{07FB10A6-0191-4D30-B709-7FAA27DC4C4F}"/>
+    <workbookView xWindow="2970" yWindow="3225" windowWidth="21600" windowHeight="11325" xr2:uid="{07FB10A6-0191-4D30-B709-7FAA27DC4C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3576,7 +3576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365E71B-710A-45EC-968B-0FFF09B2157D}">
   <dimension ref="A1:D529"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -11000,8 +11000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2F827-19C8-4524-B245-0C1FD84D892D}">
   <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E361"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>